<commit_message>
added move classification and bug fixes
</commit_message>
<xml_diff>
--- a/monopoly_app/rules.xlsx
+++ b/monopoly_app/rules.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sabesan S\Documents\Projects\monopoly_app\monopoly_api\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sabesan S\Documents\Projects\monopoly_app\monopoly_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836C9D3E-DEE9-4172-BAB5-46A9CF166A51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D898941-BDB7-486C-9393-CE2B97E2BC63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1C3FD159-372D-4F3C-8FAE-9DC01D4456BE}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1C3FD159-372D-4F3C-8FAE-9DC01D4456BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="53">
   <si>
     <t>Properties</t>
   </si>
@@ -161,13 +161,50 @@
   </si>
   <si>
     <t>Resource not found</t>
+  </si>
+  <si>
+    <t>Notification</t>
+  </si>
+  <si>
+    <t>Notification Audience</t>
+  </si>
+  <si>
+    <t>Move Classification</t>
+  </si>
+  <si>
+    <t>NoActionPlacement</t>
+  </si>
+  <si>
+    <t>Everyone</t>
+  </si>
+  <si>
+    <t>SinglePaymentRequired(Total Cost of Rent)
+MultiplePaymentRequired(Total Cost of Rent)</t>
+  </si>
+  <si>
+    <t>GainCards</t>
+  </si>
+  <si>
+    <t>MultiplePaymentRequired(Total Cost of Card)</t>
+  </si>
+  <si>
+    <t>SinglePaymentRequired(Total Cost of Card)</t>
+  </si>
+  <si>
+    <t>CancelActionPlacement</t>
+  </si>
+  <si>
+    <t>ForcedStealPlacement</t>
+  </si>
+  <si>
+    <t>ForcedStealSetPlacement</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,13 +212,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -196,11 +246,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC16AB09-DEC6-42F7-BEDC-52C8BB4ED82E}">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12:D13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -528,29 +579,41 @@
     <col min="4" max="4" width="64.21875" customWidth="1"/>
     <col min="5" max="5" width="31.77734375" customWidth="1"/>
     <col min="6" max="6" width="47" customWidth="1"/>
+    <col min="7" max="7" width="44.44140625" customWidth="1"/>
+    <col min="8" max="8" width="26.5546875" customWidth="1"/>
+    <col min="9" max="9" width="26.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -566,8 +629,14 @@
       <c r="F2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>2</v>
       </c>
@@ -580,8 +649,14 @@
       <c r="F3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -597,8 +672,14 @@
       <c r="F4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>2</v>
       </c>
@@ -611,8 +692,14 @@
       <c r="F5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="G5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -628,8 +715,11 @@
       <c r="F6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>7</v>
       </c>
@@ -642,8 +732,11 @@
       <c r="F7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>20</v>
       </c>
@@ -656,8 +749,11 @@
       <c r="F8" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -676,8 +772,11 @@
       <c r="F9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>7</v>
       </c>
@@ -690,8 +789,11 @@
       <c r="F10" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
         <v>20</v>
       </c>
@@ -704,8 +806,11 @@
       <c r="F11" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -724,8 +829,11 @@
       <c r="F12" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>7</v>
       </c>
@@ -738,8 +846,11 @@
       <c r="F13" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>20</v>
       </c>
@@ -752,8 +863,11 @@
       <c r="F14" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -772,8 +886,11 @@
       <c r="F15" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G15" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
         <v>7</v>
       </c>
@@ -786,8 +903,11 @@
       <c r="F16" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
         <v>20</v>
       </c>
@@ -800,8 +920,11 @@
       <c r="F17" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -820,8 +943,11 @@
       <c r="F18" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
         <v>7</v>
       </c>
@@ -834,8 +960,11 @@
       <c r="F19" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
         <v>20</v>
       </c>
@@ -848,8 +977,11 @@
       <c r="F20" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -868,8 +1000,11 @@
       <c r="F21" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
         <v>7</v>
       </c>
@@ -882,8 +1017,11 @@
       <c r="F22" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
         <v>20</v>
       </c>
@@ -896,8 +1034,11 @@
       <c r="F23" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -916,8 +1057,11 @@
       <c r="F24" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
         <v>20</v>
       </c>
@@ -930,8 +1074,11 @@
       <c r="F25" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
         <v>9</v>
       </c>
@@ -944,8 +1091,11 @@
       <c r="F26" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -964,8 +1114,11 @@
       <c r="F27" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C28" t="s">
         <v>7</v>
       </c>
@@ -978,8 +1131,11 @@
       <c r="F28" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C29" t="s">
         <v>20</v>
       </c>
@@ -992,8 +1148,11 @@
       <c r="F29" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G29" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -1012,8 +1171,11 @@
       <c r="F30" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G30" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C31" t="s">
         <v>7</v>
       </c>
@@ -1026,8 +1188,11 @@
       <c r="F31" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G31" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C32" t="s">
         <v>20</v>
       </c>
@@ -1040,8 +1205,11 @@
       <c r="F32" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G32" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -1060,8 +1228,11 @@
       <c r="F33" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G33" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C34" t="s">
         <v>7</v>
       </c>
@@ -1074,8 +1245,11 @@
       <c r="F34" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G34" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C35" t="s">
         <v>20</v>
       </c>
@@ -1087,6 +1261,9 @@
       </c>
       <c r="F35" t="s">
         <v>3</v>
+      </c>
+      <c r="G35" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added game play action resource
</commit_message>
<xml_diff>
--- a/monopoly_app/rules.xlsx
+++ b/monopoly_app/rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sabesan S\Documents\Projects\monopoly_app\monopoly_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D898941-BDB7-486C-9393-CE2B97E2BC63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{072C7827-1170-4CC7-8ABB-9B268F5AC6FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1C3FD159-372D-4F3C-8FAE-9DC01D4456BE}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="54">
   <si>
     <t>Properties</t>
   </si>
@@ -198,6 +198,10 @@
   </si>
   <si>
     <t>ForcedStealSetPlacement</t>
+  </si>
+  <si>
+    <t>1. Pick player or players to pay rent
+2. Or check to see if double card is avaialable to end the turn</t>
   </si>
 </sst>
 </file>
@@ -568,8 +572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC16AB09-DEC6-42F7-BEDC-52C8BB4ED82E}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -709,8 +713,8 @@
       <c r="D6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E6" t="s">
-        <v>25</v>
+      <c r="E6" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="F6" t="s">
         <v>26</v>

</xml_diff>